<commit_message>
added entidad codes, and visualization options
</commit_message>
<xml_diff>
--- a/data/raw/guardia_2019.xlsx
+++ b/data/raw/guardia_2019.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipesn/Documents/R/despliegue-guardia/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipesn/Documents/R/despliegue_guardia_nacional/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C15AB4EB-6792-414A-9038-E1EF02116D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293E23F4-98B0-624D-A008-0AB2088CDD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="1660" windowWidth="27240" windowHeight="15940" xr2:uid="{5345AA4B-9F57-7449-BA50-C0482E02E392}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
-  <si>
-    <t>Total mensual</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Zacatecas</t>
   </si>
@@ -235,13 +232,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,906 +562,874 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2899877-7D51-7941-8574-045AB032D09D}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="6" customWidth="1"/>
-    <col min="2" max="8" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="18.1640625" style="5" customWidth="1"/>
+    <col min="2" max="8" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="2">
         <v>393</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>393</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>393</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>393</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>393</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C3" s="2">
         <v>747</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>747</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>747</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>747</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>747</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>1888</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="2">
         <v>433</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>433</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>433</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>433</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>433</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>842</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C5" s="2">
         <v>479</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>479</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>479</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>479</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>479</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>874</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C6" s="2">
         <v>2424</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>2424</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>2424</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>2424</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>2424</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>3369</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C7" s="4">
         <v>1589</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1589</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1589</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1589</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>1589</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>2025</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C8" s="2">
         <v>1338</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1338</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1338</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>1338</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>1338</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>1438</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C9" s="2">
         <v>535</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>535</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>535</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>535</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>535</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>902</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C10" s="4">
         <v>3047</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3047</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3047</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>3047</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>3047</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>3442</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C11" s="2">
         <v>792</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>792</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>792</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>792</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>792</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>680</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C12" s="2">
         <v>2110</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>2110</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>2110</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>2110</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>2110</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>3326</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="2">
         <v>2538</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>2538</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>2538</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>2538</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>2538</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>3311</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C14" s="2">
         <v>1608</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1608</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>1608</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>1608</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>1608</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>2043</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C15" s="2">
         <v>3470</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>3470</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>3470</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>3470</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>3470</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>3848</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C16" s="4">
         <v>9141</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>9141</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>9141</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>9141</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>9141</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>8579</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C17" s="2">
         <v>3628</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>3628</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>3628</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>3628</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>3628</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>4362</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="2">
         <v>791</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>791</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>791</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>791</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>791</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>1397</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C19" s="2">
         <v>664</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>664</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>664</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>664</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>664</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>977</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C20" s="2">
         <v>1766</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>1766</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1766</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>1766</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>1766</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>2131</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C21" s="2">
         <v>3391</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>3391</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>3391</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>3391</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>3391</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>4323</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C22" s="3">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C22" s="2">
         <v>2163</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>2163</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>2163</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>2163</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>2163</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>3066</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C23" s="2">
         <v>1260</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>1260</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>1260</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>1260</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>1260</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>1782</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C24" s="3">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C24" s="2">
         <v>1453</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>1453</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>1453</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>1453</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>1453</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>1994</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C25" s="3">
+      <c r="A25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C25" s="2">
         <v>874</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>874</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>874</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>874</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>874</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>1231</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C26" s="2">
         <v>941</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>941</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>941</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>941</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>941</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>1662</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C27" s="2">
         <v>1186</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>1186</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1186</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>1186</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>1186</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>2621</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C28" s="3">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C28" s="2">
         <v>1116</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>1116</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>1116</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>1116</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>1116</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>1587</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C29" s="3">
+      <c r="A29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C29" s="2">
         <v>1215</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>1215</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>1215</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>1215</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>1215</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>2912</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C30" s="3">
+      <c r="A30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C30" s="2">
         <v>410</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>410</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>410</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>410</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>410</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>697</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C31" s="3">
+      <c r="A31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C31" s="2">
         <v>2458</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>2458</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>2458</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>2458</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>2458</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>4198</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C32" s="3">
+      <c r="A32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C32" s="2">
         <v>673</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>673</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>673</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>673</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>673</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>759</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C33" s="3">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C33" s="2">
         <v>1558</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>1558</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>1558</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>1558</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>1558</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>1647</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C34" s="3">
-        <f>SUM(C2:C33)</f>
-        <v>56191</v>
-      </c>
-      <c r="D34" s="3">
-        <f>SUM(D2:D33)</f>
-        <v>56191</v>
-      </c>
-      <c r="E34" s="3">
-        <f>SUM(E2:E33)</f>
-        <v>56191</v>
-      </c>
-      <c r="F34" s="3">
-        <f>SUM(F2:F33)</f>
-        <v>56191</v>
-      </c>
-      <c r="G34" s="3">
-        <f>SUM(G2:G33)</f>
-        <v>56191</v>
-      </c>
-      <c r="H34" s="3">
-        <f>SUM(H2:H33)</f>
-        <v>74437</v>
       </c>
     </row>
   </sheetData>
@@ -1521,8 +1483,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B34 H2:H33">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="B1">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1531,8 +1493,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B2:B33 H2:H33">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>